<commit_message>
Asignación de autores Mat 8 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="264">
   <si>
     <t>Asignatura</t>
   </si>
@@ -913,6 +913,15 @@
   </si>
   <si>
     <t>Identifica los distintos tipos de rectas</t>
+  </si>
+  <si>
+    <t>Andrea Sabogal</t>
+  </si>
+  <si>
+    <t>Diana Gonzalez</t>
+  </si>
+  <si>
+    <t>Cristhian Fuentes</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1090,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1156,11 +1165,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1269,16 +1287,79 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1320,67 +1401,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1689,9 +1713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,65 +1746,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="63" t="s">
+      <c r="S1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="61" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="38" t="s">
@@ -1789,36 +1813,36 @@
       <c r="W1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="X1" s="80" t="s">
+      <c r="X1" s="55" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="51"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="9" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1836,52 +1860,52 @@
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="H3" s="69">
+      <c r="H3" s="44">
         <v>1</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="69" t="s">
+      <c r="K3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="L3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83" t="s">
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="71">
+      <c r="Q3" s="46">
         <v>10</v>
       </c>
-      <c r="R3" s="71" t="s">
+      <c r="R3" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="S3" s="72" t="s">
+      <c r="S3" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T3" s="72" t="s">
+      <c r="T3" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="U3" s="71" t="s">
+      <c r="U3" s="46" t="s">
         <v>220</v>
       </c>
       <c r="V3" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W3" s="73">
+      <c r="W3" s="48">
         <v>42394</v>
       </c>
-      <c r="X3" s="81">
+      <c r="X3" s="56">
         <v>42394</v>
       </c>
     </row>
@@ -1942,6 +1966,9 @@
       </c>
       <c r="U4" s="20" t="s">
         <v>195</v>
+      </c>
+      <c r="V4" s="84" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -1998,6 +2025,9 @@
       <c r="U5" s="20" t="s">
         <v>197</v>
       </c>
+      <c r="V5" s="84" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -2057,6 +2087,9 @@
       <c r="U6" s="20" t="s">
         <v>201</v>
       </c>
+      <c r="V6" s="84" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -2116,6 +2149,9 @@
       <c r="U7" s="20" t="s">
         <v>195</v>
       </c>
+      <c r="V7" s="84" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
@@ -2177,6 +2213,9 @@
       <c r="U8" s="20" t="s">
         <v>195</v>
       </c>
+      <c r="V8" s="84" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -2193,54 +2232,54 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="74" t="s">
+      <c r="G9" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="75">
+      <c r="H9" s="50">
         <v>7</v>
       </c>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="74" t="s">
+      <c r="J9" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="K9" s="76" t="s">
+      <c r="K9" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="76" t="s">
+      <c r="L9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="74" t="s">
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="P9" s="77" t="s">
+      <c r="P9" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="77">
+      <c r="Q9" s="52">
         <v>10</v>
       </c>
-      <c r="R9" s="77" t="s">
+      <c r="R9" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="S9" s="78" t="s">
+      <c r="S9" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="T9" s="78" t="s">
+      <c r="T9" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="U9" s="77" t="s">
+      <c r="U9" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="V9" s="79" t="s">
+      <c r="V9" s="54" t="s">
         <v>245</v>
       </c>
       <c r="Y9" t="s">
         <v>257</v>
       </c>
-      <c r="AB9" s="67">
+      <c r="AB9" s="42">
         <v>42547</v>
       </c>
     </row>
@@ -2259,54 +2298,54 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="74" t="s">
+      <c r="G10" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="52">
         <v>8</v>
       </c>
-      <c r="I10" s="76" t="s">
+      <c r="I10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="74" t="s">
+      <c r="J10" s="49" t="s">
         <v>229</v>
       </c>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="76" t="s">
+      <c r="L10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="74" t="s">
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="P10" s="77" t="s">
+      <c r="P10" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="77">
+      <c r="Q10" s="52">
         <v>10</v>
       </c>
-      <c r="R10" s="77" t="s">
+      <c r="R10" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="S10" s="78" t="s">
+      <c r="S10" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="T10" s="78" t="s">
+      <c r="T10" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="U10" s="77" t="s">
+      <c r="U10" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="V10" s="79" t="s">
+      <c r="V10" s="54" t="s">
         <v>245</v>
       </c>
       <c r="Y10" t="s">
         <v>253</v>
       </c>
-      <c r="AB10" s="67">
+      <c r="AB10" s="42">
         <v>42395</v>
       </c>
     </row>
@@ -2325,49 +2364,49 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="68" t="s">
+      <c r="G11" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="44">
         <v>9</v>
       </c>
-      <c r="I11" s="70" t="s">
+      <c r="I11" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K11" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="70" t="s">
+      <c r="L11" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="71" t="s">
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="71">
+      <c r="Q11" s="46">
         <v>10</v>
       </c>
-      <c r="R11" s="71" t="s">
+      <c r="R11" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="S11" s="72" t="s">
+      <c r="S11" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T11" s="72" t="s">
+      <c r="T11" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="U11" s="71" t="s">
+      <c r="U11" s="46" t="s">
         <v>220</v>
       </c>
       <c r="V11" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W11" s="73">
+      <c r="W11" s="48">
         <v>42395</v>
       </c>
       <c r="X11" t="s">
@@ -2389,49 +2428,49 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="46">
         <v>10</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="68" t="s">
+      <c r="J12" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="K12" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="70" t="s">
+      <c r="L12" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="71" t="s">
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="71">
+      <c r="Q12" s="46">
         <v>10</v>
       </c>
-      <c r="R12" s="71" t="s">
+      <c r="R12" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="S12" s="72" t="s">
+      <c r="S12" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T12" s="72" t="s">
+      <c r="T12" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="U12" s="71" t="s">
+      <c r="U12" s="46" t="s">
         <v>217</v>
       </c>
       <c r="V12" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W12" s="73">
+      <c r="W12" s="48">
         <v>42761</v>
       </c>
       <c r="X12" t="s">
@@ -2456,43 +2495,43 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="74" t="s">
+      <c r="G13" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="H13" s="75">
+      <c r="H13" s="50">
         <v>11</v>
       </c>
-      <c r="I13" s="76" t="s">
+      <c r="I13" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="74" t="s">
+      <c r="J13" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="K13" s="76" t="s">
+      <c r="K13" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="76" t="s">
+      <c r="L13" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="76"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="77" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="77">
+      <c r="Q13" s="52">
         <v>10</v>
       </c>
-      <c r="R13" s="77" t="s">
+      <c r="R13" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="S13" s="78" t="s">
+      <c r="S13" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="T13" s="78" t="s">
+      <c r="T13" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="U13" s="77" t="s">
+      <c r="U13" s="52" t="s">
         <v>217</v>
       </c>
       <c r="V13" s="41" t="s">
@@ -2523,49 +2562,49 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="71">
+      <c r="H14" s="46">
         <v>12</v>
       </c>
-      <c r="I14" s="70" t="s">
+      <c r="I14" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="68" t="s">
+      <c r="J14" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="K14" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="70" t="s">
+      <c r="L14" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="71" t="s">
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="71">
+      <c r="Q14" s="46">
         <v>10</v>
       </c>
-      <c r="R14" s="71" t="s">
+      <c r="R14" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="S14" s="72" t="s">
+      <c r="S14" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T14" s="72" t="s">
+      <c r="T14" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="U14" s="71" t="s">
+      <c r="U14" s="46" t="s">
         <v>217</v>
       </c>
       <c r="V14" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W14" s="73">
+      <c r="W14" s="48">
         <v>42395</v>
       </c>
       <c r="X14" t="s">
@@ -2587,49 +2626,49 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="68" t="s">
+      <c r="G15" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="69">
+      <c r="H15" s="44">
         <v>13</v>
       </c>
-      <c r="I15" s="70" t="s">
+      <c r="I15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="68" t="s">
+      <c r="J15" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="K15" s="70" t="s">
+      <c r="K15" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="70" t="s">
+      <c r="L15" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="70"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="71" t="s">
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="71">
+      <c r="Q15" s="46">
         <v>10</v>
       </c>
-      <c r="R15" s="71" t="s">
+      <c r="R15" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="S15" s="72" t="s">
+      <c r="S15" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T15" s="72" t="s">
+      <c r="T15" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="U15" s="71" t="s">
+      <c r="U15" s="46" t="s">
         <v>220</v>
       </c>
       <c r="V15" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W15" s="73">
+      <c r="W15" s="48">
         <v>42395</v>
       </c>
       <c r="X15" t="s">
@@ -2651,49 +2690,49 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="46">
         <v>14</v>
       </c>
-      <c r="I16" s="70" t="s">
+      <c r="I16" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="68" t="s">
+      <c r="J16" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="K16" s="70" t="s">
+      <c r="K16" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="70" t="s">
+      <c r="L16" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="68"/>
-      <c r="P16" s="71" t="s">
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="71">
+      <c r="Q16" s="46">
         <v>10</v>
       </c>
-      <c r="R16" s="71" t="s">
+      <c r="R16" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="S16" s="72" t="s">
+      <c r="S16" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T16" s="72" t="s">
+      <c r="T16" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="U16" s="71" t="s">
+      <c r="U16" s="46" t="s">
         <v>222</v>
       </c>
       <c r="V16" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W16" s="73">
+      <c r="W16" s="48">
         <v>42395</v>
       </c>
       <c r="X16" t="s">
@@ -2715,49 +2754,49 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="68" t="s">
+      <c r="G17" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="H17" s="69">
+      <c r="H17" s="44">
         <v>15</v>
       </c>
-      <c r="I17" s="70" t="s">
+      <c r="I17" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="68" t="s">
+      <c r="J17" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="70" t="s">
+      <c r="L17" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="68"/>
-      <c r="P17" s="71" t="s">
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="71">
+      <c r="Q17" s="46">
         <v>10</v>
       </c>
-      <c r="R17" s="71" t="s">
+      <c r="R17" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="S17" s="72" t="s">
+      <c r="S17" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T17" s="72" t="s">
+      <c r="T17" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="U17" s="71" t="s">
+      <c r="U17" s="46" t="s">
         <v>217</v>
       </c>
       <c r="V17" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W17" s="73">
+      <c r="W17" s="48">
         <v>42395</v>
       </c>
       <c r="X17" t="s">
@@ -2779,43 +2818,43 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="74" t="s">
+      <c r="G18" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="H18" s="77">
+      <c r="H18" s="52">
         <v>16</v>
       </c>
-      <c r="I18" s="76" t="s">
+      <c r="I18" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="K18" s="76" t="s">
+      <c r="K18" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="76" t="s">
+      <c r="L18" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="77" t="s">
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="77">
+      <c r="Q18" s="52">
         <v>10</v>
       </c>
-      <c r="R18" s="77" t="s">
+      <c r="R18" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="S18" s="78" t="s">
+      <c r="S18" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="T18" s="78" t="s">
+      <c r="T18" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="U18" s="77" t="s">
+      <c r="U18" s="52" t="s">
         <v>217</v>
       </c>
       <c r="V18" s="41" t="s">
@@ -2846,43 +2885,43 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="74" t="s">
+      <c r="G19" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="75">
+      <c r="H19" s="50">
         <v>17</v>
       </c>
-      <c r="I19" s="76" t="s">
+      <c r="I19" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="74" t="s">
+      <c r="J19" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="K19" s="76" t="s">
+      <c r="K19" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="76" t="s">
+      <c r="L19" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="77" t="s">
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="77">
+      <c r="Q19" s="52">
         <v>10</v>
       </c>
-      <c r="R19" s="77" t="s">
+      <c r="R19" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="S19" s="78" t="s">
+      <c r="S19" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="T19" s="78" t="s">
+      <c r="T19" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="U19" s="77" t="s">
+      <c r="U19" s="52" t="s">
         <v>222</v>
       </c>
       <c r="V19" s="41" t="s">
@@ -2913,49 +2952,49 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="H20" s="71">
+      <c r="H20" s="46">
         <v>18</v>
       </c>
-      <c r="I20" s="70" t="s">
+      <c r="I20" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="68" t="s">
+      <c r="J20" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="K20" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="70" t="s">
+      <c r="L20" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="71" t="s">
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="71">
+      <c r="Q20" s="46">
         <v>10</v>
       </c>
-      <c r="R20" s="71" t="s">
+      <c r="R20" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="S20" s="72" t="s">
+      <c r="S20" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T20" s="72" t="s">
+      <c r="T20" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="U20" s="71" t="s">
+      <c r="U20" s="46" t="s">
         <v>222</v>
       </c>
       <c r="V20" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W20" s="73">
+      <c r="W20" s="48">
         <v>42395</v>
       </c>
       <c r="X20" t="s">
@@ -2977,49 +3016,49 @@
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="H21" s="69">
+      <c r="H21" s="44">
         <v>19</v>
       </c>
-      <c r="I21" s="70" t="s">
+      <c r="I21" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="68" t="s">
+      <c r="J21" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="K21" s="70" t="s">
+      <c r="K21" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="70" t="s">
+      <c r="L21" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="68"/>
-      <c r="P21" s="71" t="s">
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="71">
+      <c r="Q21" s="46">
         <v>10</v>
       </c>
-      <c r="R21" s="71" t="s">
+      <c r="R21" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="S21" s="72" t="s">
+      <c r="S21" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T21" s="72" t="s">
+      <c r="T21" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="U21" s="71" t="s">
+      <c r="U21" s="46" t="s">
         <v>222</v>
       </c>
       <c r="V21" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W21" s="73">
+      <c r="W21" s="48">
         <v>42395</v>
       </c>
       <c r="X21" t="s">
@@ -3041,51 +3080,51 @@
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="71">
+      <c r="H22" s="46">
         <v>20</v>
       </c>
-      <c r="I22" s="70" t="s">
+      <c r="I22" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="K22" s="70" t="s">
+      <c r="K22" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="70" t="s">
+      <c r="L22" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="68" t="s">
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="P22" s="71" t="s">
+      <c r="P22" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="71">
+      <c r="Q22" s="46">
         <v>10</v>
       </c>
-      <c r="R22" s="71" t="s">
+      <c r="R22" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="S22" s="72" t="s">
+      <c r="S22" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="T22" s="72" t="s">
+      <c r="T22" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="U22" s="71" t="s">
+      <c r="U22" s="46" t="s">
         <v>222</v>
       </c>
       <c r="V22" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="W22" s="73">
+      <c r="W22" s="48">
         <v>42395</v>
       </c>
       <c r="X22" t="s">
@@ -3210,6 +3249,9 @@
       <c r="U24" s="12" t="s">
         <v>195</v>
       </c>
+      <c r="V24" s="84" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
@@ -3559,6 +3601,9 @@
       <c r="U30" s="28" t="s">
         <v>201</v>
       </c>
+      <c r="V30" s="40" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
@@ -3734,6 +3779,9 @@
       <c r="U33" s="28" t="s">
         <v>197</v>
       </c>
+      <c r="V33" s="40" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
@@ -3956,6 +4004,9 @@
       <c r="U37" s="34" t="s">
         <v>195</v>
       </c>
+      <c r="V37" s="85" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="38" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -4014,6 +4065,9 @@
       </c>
       <c r="U38" s="34" t="s">
         <v>195</v>
+      </c>
+      <c r="V38" s="85" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -5183,12 +5237,6 @@
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5203,6 +5251,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Autores de recursos mat 8 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -1713,9 +1713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W38" sqref="W38"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,15 +1729,15 @@
     <col min="7" max="7" width="64.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="74.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42.28515625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="74.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="23" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="42.28515625" style="11" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="56.5703125" style="11" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
Actualización estado de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="264">
   <si>
     <t>Asignatura</t>
   </si>
@@ -915,10 +915,13 @@
     <t>faltan 10</t>
   </si>
   <si>
-    <t>proceso 6</t>
-  </si>
-  <si>
     <t>proceso 1</t>
+  </si>
+  <si>
+    <t>Listos 26</t>
+  </si>
+  <si>
+    <t>Faltan 10</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1331,20 +1334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1389,16 +1378,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1439,49 +1471,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1789,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomLeft" activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,65 +1812,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="73"/>
+      <c r="O1" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="67" t="s">
+      <c r="U1" s="53" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="22" t="s">
@@ -1890,36 +1879,36 @@
       <c r="W1" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="X1" s="26" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="68"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="9"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1937,52 +1926,52 @@
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="36">
         <v>1</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="44" t="s">
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="45">
+      <c r="Q3" s="39">
         <v>10</v>
       </c>
-      <c r="R3" s="45" t="s">
+      <c r="R3" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="S3" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="T3" s="46" t="s">
+      <c r="T3" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="U3" s="45" t="s">
+      <c r="U3" s="39" t="s">
         <v>219</v>
       </c>
       <c r="V3" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W3" s="41">
+      <c r="W3" s="35">
         <v>42394</v>
       </c>
-      <c r="X3" s="33">
+      <c r="X3" s="27">
         <v>42394</v>
       </c>
     </row>
@@ -2038,13 +2027,13 @@
       <c r="S4" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T4" s="47" t="s">
+      <c r="T4" s="41" t="s">
         <v>193</v>
       </c>
       <c r="U4" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V4" s="34" t="s">
+      <c r="V4" s="28" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2066,7 +2055,7 @@
       <c r="G5" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="48">
+      <c r="H5" s="42">
         <v>3</v>
       </c>
       <c r="I5" s="12" t="s">
@@ -2096,13 +2085,13 @@
       <c r="S5" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="T5" s="47" t="s">
+      <c r="T5" s="41" t="s">
         <v>204</v>
       </c>
       <c r="U5" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="V5" s="34" t="s">
+      <c r="V5" s="28" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2158,13 +2147,13 @@
       <c r="S6" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="T6" s="41" t="s">
         <v>199</v>
       </c>
       <c r="U6" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="V6" s="34" t="s">
+      <c r="V6" s="28" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2186,7 +2175,7 @@
       <c r="G7" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="42">
         <v>5</v>
       </c>
       <c r="I7" s="12" t="s">
@@ -2220,13 +2209,13 @@
       <c r="S7" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="41" t="s">
         <v>193</v>
       </c>
       <c r="U7" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V7" s="34" t="s">
+      <c r="V7" s="28" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2284,13 +2273,13 @@
       <c r="S8" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T8" s="47" t="s">
+      <c r="T8" s="41" t="s">
         <v>201</v>
       </c>
       <c r="U8" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V8" s="34" t="s">
+      <c r="V8" s="28" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2309,54 +2298,54 @@
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="30">
         <v>7</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="37" t="s">
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="P9" s="38" t="s">
+      <c r="P9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="32">
         <v>10</v>
       </c>
-      <c r="R9" s="38" t="s">
+      <c r="R9" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S9" s="40" t="s">
+      <c r="S9" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T9" s="40" t="s">
+      <c r="T9" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="U9" s="38" t="s">
+      <c r="U9" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V9" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W9" s="34" t="s">
+      <c r="W9" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="X9" s="34" t="s">
+      <c r="X9" s="28" t="s">
         <v>249</v>
       </c>
       <c r="AB9" s="25"/>
@@ -2376,54 +2365,54 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="32">
         <v>8</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="K10" s="39" t="s">
+      <c r="K10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="37" t="s">
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="P10" s="38" t="s">
+      <c r="P10" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="32">
         <v>10</v>
       </c>
-      <c r="R10" s="38" t="s">
+      <c r="R10" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S10" s="40" t="s">
+      <c r="S10" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T10" s="40" t="s">
+      <c r="T10" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="U10" s="38" t="s">
+      <c r="U10" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V10" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W10" s="34" t="s">
+      <c r="W10" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="X10" s="34" t="s">
+      <c r="X10" s="28" t="s">
         <v>249</v>
       </c>
       <c r="Y10" t="s">
@@ -2446,49 +2435,49 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="30">
         <v>9</v>
       </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="38" t="s">
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="32">
         <v>10</v>
       </c>
-      <c r="R11" s="38" t="s">
+      <c r="R11" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="S11" s="40" t="s">
+      <c r="S11" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T11" s="40" t="s">
+      <c r="T11" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="U11" s="38" t="s">
+      <c r="U11" s="32" t="s">
         <v>219</v>
       </c>
       <c r="V11" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W11" s="41">
+      <c r="W11" s="35">
         <v>42395</v>
       </c>
       <c r="X11" t="s">
@@ -2510,49 +2499,49 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="32">
         <v>10</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="J12" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="K12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="38" t="s">
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="32">
         <v>10</v>
       </c>
-      <c r="R12" s="38" t="s">
+      <c r="R12" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S12" s="40" t="s">
+      <c r="S12" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T12" s="40" t="s">
+      <c r="T12" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="U12" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V12" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W12" s="41">
+      <c r="W12" s="35">
         <v>42761</v>
       </c>
       <c r="X12" t="s">
@@ -2574,43 +2563,43 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="30">
         <v>11</v>
       </c>
-      <c r="I13" s="39" t="s">
+      <c r="I13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="38" t="s">
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="32">
         <v>10</v>
       </c>
-      <c r="R13" s="38" t="s">
+      <c r="R13" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S13" s="40" t="s">
+      <c r="S13" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T13" s="40" t="s">
+      <c r="T13" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="U13" s="38" t="s">
+      <c r="U13" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V13" s="24" t="s">
@@ -2641,49 +2630,49 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="32">
         <v>12</v>
       </c>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="37" t="s">
+      <c r="J14" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="38" t="s">
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="32">
         <v>10</v>
       </c>
-      <c r="R14" s="38" t="s">
+      <c r="R14" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S14" s="40" t="s">
+      <c r="S14" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T14" s="40" t="s">
+      <c r="T14" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V14" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W14" s="41">
+      <c r="W14" s="35">
         <v>42395</v>
       </c>
       <c r="X14" t="s">
@@ -2705,49 +2694,49 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="30">
         <v>13</v>
       </c>
-      <c r="I15" s="39" t="s">
+      <c r="I15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="38" t="s">
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="38">
+      <c r="Q15" s="32">
         <v>10</v>
       </c>
-      <c r="R15" s="38" t="s">
+      <c r="R15" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="S15" s="40" t="s">
+      <c r="S15" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T15" s="40" t="s">
+      <c r="T15" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="U15" s="38" t="s">
+      <c r="U15" s="32" t="s">
         <v>219</v>
       </c>
       <c r="V15" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W15" s="41">
+      <c r="W15" s="35">
         <v>42395</v>
       </c>
       <c r="X15" t="s">
@@ -2769,49 +2758,49 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="32">
         <v>14</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="I16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="K16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="39" t="s">
+      <c r="L16" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="38" t="s">
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="32">
         <v>10</v>
       </c>
-      <c r="R16" s="38" t="s">
+      <c r="R16" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S16" s="40" t="s">
+      <c r="S16" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T16" s="40" t="s">
+      <c r="T16" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="U16" s="38" t="s">
+      <c r="U16" s="32" t="s">
         <v>221</v>
       </c>
       <c r="V16" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W16" s="41">
+      <c r="W16" s="35">
         <v>42395</v>
       </c>
       <c r="X16" t="s">
@@ -2833,49 +2822,49 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="30">
         <v>15</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="38" t="s">
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="38">
+      <c r="Q17" s="32">
         <v>10</v>
       </c>
-      <c r="R17" s="38" t="s">
+      <c r="R17" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S17" s="40" t="s">
+      <c r="S17" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T17" s="40" t="s">
+      <c r="T17" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="U17" s="38" t="s">
+      <c r="U17" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V17" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W17" s="41">
+      <c r="W17" s="35">
         <v>42395</v>
       </c>
       <c r="X17" t="s">
@@ -2897,43 +2886,43 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="32">
         <v>16</v>
       </c>
-      <c r="I18" s="39" t="s">
+      <c r="I18" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="K18" s="39" t="s">
+      <c r="K18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="38" t="s">
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="32">
         <v>10</v>
       </c>
-      <c r="R18" s="38" t="s">
+      <c r="R18" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S18" s="40" t="s">
+      <c r="S18" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T18" s="40" t="s">
+      <c r="T18" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="U18" s="38" t="s">
+      <c r="U18" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V18" s="24" t="s">
@@ -2964,43 +2953,43 @@
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="30">
         <v>17</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K19" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="38" t="s">
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="32">
         <v>10</v>
       </c>
-      <c r="R19" s="38" t="s">
+      <c r="R19" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T19" s="40" t="s">
+      <c r="T19" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="U19" s="38" t="s">
+      <c r="U19" s="32" t="s">
         <v>221</v>
       </c>
       <c r="V19" s="24" t="s">
@@ -3031,49 +3020,49 @@
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="32">
         <v>18</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="37" t="s">
+      <c r="J20" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="39" t="s">
+      <c r="L20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="38" t="s">
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="38">
+      <c r="Q20" s="32">
         <v>10</v>
       </c>
-      <c r="R20" s="38" t="s">
+      <c r="R20" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S20" s="40" t="s">
+      <c r="S20" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T20" s="40" t="s">
+      <c r="T20" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="U20" s="38" t="s">
+      <c r="U20" s="32" t="s">
         <v>221</v>
       </c>
       <c r="V20" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W20" s="41">
+      <c r="W20" s="35">
         <v>42395</v>
       </c>
       <c r="X20" t="s">
@@ -3095,49 +3084,49 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="30">
         <v>19</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="K21" s="39" t="s">
+      <c r="K21" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="39" t="s">
+      <c r="L21" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="38" t="s">
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="38">
+      <c r="Q21" s="32">
         <v>10</v>
       </c>
-      <c r="R21" s="38" t="s">
+      <c r="R21" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S21" s="40" t="s">
+      <c r="S21" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T21" s="40" t="s">
+      <c r="T21" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="U21" s="38" t="s">
+      <c r="U21" s="32" t="s">
         <v>221</v>
       </c>
       <c r="V21" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W21" s="41">
+      <c r="W21" s="35">
         <v>42395</v>
       </c>
       <c r="X21" t="s">
@@ -3159,51 +3148,51 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="32">
         <v>20</v>
       </c>
-      <c r="I22" s="39" t="s">
+      <c r="I22" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="37" t="s">
+      <c r="J22" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="K22" s="39" t="s">
+      <c r="K22" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="39" t="s">
+      <c r="L22" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="37" t="s">
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="P22" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="38">
+      <c r="Q22" s="32">
         <v>10</v>
       </c>
-      <c r="R22" s="38" t="s">
+      <c r="R22" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="S22" s="40" t="s">
+      <c r="S22" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T22" s="40" t="s">
+      <c r="T22" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="U22" s="38" t="s">
+      <c r="U22" s="32" t="s">
         <v>221</v>
       </c>
       <c r="V22" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W22" s="41">
+      <c r="W22" s="35">
         <v>42395</v>
       </c>
       <c r="X22" t="s">
@@ -3225,49 +3214,49 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="30">
         <v>21</v>
       </c>
-      <c r="I23" s="28" t="s">
+      <c r="I23" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="28" t="s">
+      <c r="L23" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="29" t="s">
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="Q23" s="32">
         <v>10</v>
       </c>
-      <c r="R23" s="29" t="s">
+      <c r="R23" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S23" s="30" t="s">
+      <c r="S23" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T23" s="30" t="s">
+      <c r="T23" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="U23" s="29" t="s">
+      <c r="U23" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V23" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W23" s="31">
+      <c r="W23" s="35">
         <v>42401</v>
       </c>
       <c r="X23" t="s">
@@ -3328,13 +3317,13 @@
       <c r="S24" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T24" s="47" t="s">
+      <c r="T24" s="41" t="s">
         <v>202</v>
       </c>
       <c r="U24" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V24" s="34" t="s">
+      <c r="V24" s="28" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3353,52 +3342,52 @@
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="30">
         <v>23</v>
       </c>
-      <c r="I25" s="39" t="s">
+      <c r="I25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="K25" s="39" t="s">
+      <c r="K25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="39" t="s">
+      <c r="L25" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="38" t="s">
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="38">
+      <c r="Q25" s="32">
         <v>10</v>
       </c>
-      <c r="R25" s="38" t="s">
+      <c r="R25" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S25" s="40" t="s">
+      <c r="S25" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T25" s="40" t="s">
+      <c r="T25" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="U25" s="38" t="s">
+      <c r="U25" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V25" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W25" s="34" t="s">
+      <c r="W25" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="X25" s="34" t="s">
+      <c r="X25" s="28" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3417,52 +3406,52 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="32">
         <v>24</v>
       </c>
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="37" t="s">
+      <c r="J26" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="K26" s="39" t="s">
+      <c r="K26" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="L26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="38" t="s">
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="Q26" s="32">
         <v>10</v>
       </c>
-      <c r="R26" s="38" t="s">
+      <c r="R26" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S26" s="40" t="s">
+      <c r="S26" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T26" s="40" t="s">
+      <c r="T26" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="38" t="s">
+      <c r="U26" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V26" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W26" s="34" t="s">
+      <c r="W26" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="X26" s="34" t="s">
+      <c r="X26" s="28" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3481,49 +3470,49 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="30">
         <v>25</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="28" t="s">
+      <c r="L27" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="29" t="s">
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="Q27" s="29">
+      <c r="Q27" s="32">
         <v>10</v>
       </c>
-      <c r="R27" s="29" t="s">
+      <c r="R27" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="S27" s="30" t="s">
+      <c r="S27" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T27" s="30" t="s">
+      <c r="T27" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="U27" s="29" t="s">
+      <c r="U27" s="32" t="s">
         <v>219</v>
       </c>
       <c r="V27" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W27" s="31">
+      <c r="W27" s="35">
         <v>42402</v>
       </c>
       <c r="X27" t="s">
@@ -3545,49 +3534,49 @@
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="32">
         <v>26</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="26" t="s">
+      <c r="J28" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="K28" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="29" t="s">
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="29">
+      <c r="Q28" s="32">
         <v>10</v>
       </c>
-      <c r="R28" s="29" t="s">
+      <c r="R28" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="S28" s="30" t="s">
+      <c r="S28" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T28" s="30" t="s">
+      <c r="T28" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="U28" s="29" t="s">
+      <c r="U28" s="32" t="s">
         <v>219</v>
       </c>
       <c r="V28" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W28" s="31">
+      <c r="W28" s="35">
         <v>42402</v>
       </c>
       <c r="X28" t="s">
@@ -3609,49 +3598,49 @@
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="30">
         <v>27</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="K29" s="28" t="s">
+      <c r="K29" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L29" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="29" t="s">
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="29">
+      <c r="Q29" s="32">
         <v>10</v>
       </c>
-      <c r="R29" s="29" t="s">
+      <c r="R29" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S29" s="30" t="s">
+      <c r="S29" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T29" s="30" t="s">
+      <c r="T29" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="U29" s="29" t="s">
+      <c r="U29" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V29" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W29" s="31">
+      <c r="W29" s="35">
         <v>42402</v>
       </c>
       <c r="X29" t="s">
@@ -3710,13 +3699,13 @@
       <c r="S30" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="T30" s="47" t="s">
+      <c r="T30" s="41" t="s">
         <v>203</v>
       </c>
       <c r="U30" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="V30" s="34" t="s">
+      <c r="V30" s="28" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3735,49 +3724,49 @@
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="26" t="s">
+      <c r="G31" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="30">
         <v>29</v>
       </c>
-      <c r="I31" s="28" t="s">
+      <c r="I31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L31" s="28" t="s">
+      <c r="L31" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="29" t="s">
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="29">
+      <c r="Q31" s="32">
         <v>10</v>
       </c>
-      <c r="R31" s="29" t="s">
+      <c r="R31" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="S31" s="30" t="s">
+      <c r="S31" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T31" s="30" t="s">
+      <c r="T31" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="U31" s="29" t="s">
+      <c r="U31" s="32" t="s">
         <v>219</v>
       </c>
       <c r="V31" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W31" s="31">
+      <c r="W31" s="35">
         <v>42403</v>
       </c>
       <c r="X31" t="s">
@@ -3799,52 +3788,52 @@
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="32">
         <v>30</v>
       </c>
-      <c r="I32" s="39" t="s">
+      <c r="I32" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="37" t="s">
+      <c r="J32" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="K32" s="39" t="s">
+      <c r="K32" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L32" s="39" t="s">
+      <c r="L32" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="38" t="s">
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="38">
+      <c r="Q32" s="32">
         <v>10</v>
       </c>
-      <c r="R32" s="38" t="s">
+      <c r="R32" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S32" s="40" t="s">
+      <c r="S32" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T32" s="40" t="s">
+      <c r="T32" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="U32" s="38" t="s">
+      <c r="U32" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V32" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W32" s="34" t="s">
+      <c r="W32" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="X32" s="34" t="s">
+      <c r="X32" s="28" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3866,7 +3855,7 @@
       <c r="G33" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="H33" s="48">
+      <c r="H33" s="42">
         <v>31</v>
       </c>
       <c r="I33" s="12" t="s">
@@ -3900,13 +3889,13 @@
       <c r="S33" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="T33" s="47" t="s">
+      <c r="T33" s="41" t="s">
         <v>227</v>
       </c>
       <c r="U33" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="V33" s="34" t="s">
+      <c r="V33" s="28" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3927,49 +3916,49 @@
         <v>136</v>
       </c>
       <c r="F34" s="18"/>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="32">
         <v>32</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="K34" s="28" t="s">
+      <c r="K34" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="L34" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="29" t="s">
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="29">
+      <c r="Q34" s="32">
         <v>10</v>
       </c>
-      <c r="R34" s="29" t="s">
+      <c r="R34" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S34" s="30" t="s">
+      <c r="S34" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T34" s="30" t="s">
+      <c r="T34" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="U34" s="29" t="s">
+      <c r="U34" s="32" t="s">
         <v>185</v>
       </c>
       <c r="V34" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="W34" s="31">
+      <c r="W34" s="35">
         <v>42402</v>
       </c>
       <c r="X34" t="s">
@@ -3991,43 +3980,43 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H35" s="30">
         <v>33</v>
       </c>
-      <c r="I35" s="39" t="s">
+      <c r="I35" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="37" t="s">
+      <c r="J35" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="K35" s="39" t="s">
+      <c r="K35" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L35" s="39" t="s">
+      <c r="L35" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="38" t="s">
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="38">
+      <c r="Q35" s="32">
         <v>10</v>
       </c>
-      <c r="R35" s="38" t="s">
+      <c r="R35" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="S35" s="40" t="s">
+      <c r="S35" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T35" s="40" t="s">
+      <c r="T35" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="U35" s="38" t="s">
+      <c r="U35" s="32" t="s">
         <v>216</v>
       </c>
       <c r="V35" s="24" t="s">
@@ -4055,37 +4044,37 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="37" t="s">
+      <c r="G36" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="32">
         <v>34</v>
       </c>
-      <c r="I36" s="39" t="s">
+      <c r="I36" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="37" t="s">
+      <c r="J36" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="K36" s="39" t="s">
+      <c r="K36" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="39" t="s">
+      <c r="L36" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="38" t="s">
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="38"/>
-      <c r="R36" s="38"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="38"/>
-      <c r="V36" s="49"/>
-      <c r="W36" s="49"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="43"/>
+      <c r="W36" s="43"/>
       <c r="X36" t="s">
         <v>249</v>
       </c>
@@ -4108,7 +4097,7 @@
       <c r="G37" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="H37" s="48">
+      <c r="H37" s="42">
         <v>35</v>
       </c>
       <c r="I37" s="12" t="s">
@@ -4142,13 +4131,13 @@
       <c r="S37" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T37" s="47" t="s">
+      <c r="T37" s="41" t="s">
         <v>193</v>
       </c>
       <c r="U37" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V37" s="35" t="s">
+      <c r="V37" s="29" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4204,13 +4193,13 @@
       <c r="S38" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="T38" s="47" t="s">
+      <c r="T38" s="41" t="s">
         <v>205</v>
       </c>
       <c r="U38" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="V38" s="35" t="s">
+      <c r="V38" s="29" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4259,6 +4248,12 @@
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
       <c r="U40" s="13"/>
+      <c r="V40" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="W40" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="41" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
@@ -4281,13 +4276,11 @@
       <c r="R41" s="13"/>
       <c r="S41" s="14"/>
       <c r="T41" s="14"/>
-      <c r="U41" s="75"/>
-      <c r="V41" s="77"/>
-      <c r="W41" s="78" t="s">
+      <c r="U41" s="44"/>
+      <c r="V41" s="46"/>
+      <c r="W41" s="47"/>
+      <c r="X41" s="48" t="s">
         <v>261</v>
-      </c>
-      <c r="X41" s="79" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4311,14 +4304,14 @@
       <c r="R42" s="11"/>
       <c r="S42" s="14"/>
       <c r="T42" s="14"/>
-      <c r="U42" s="76"/>
-      <c r="V42" s="80" t="s">
+      <c r="U42" s="45"/>
+      <c r="V42" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="W42" s="78" t="s">
+      <c r="W42" s="47" t="s">
         <v>260</v>
       </c>
-      <c r="X42" s="81" t="s">
+      <c r="X42" s="50" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5379,12 +5372,6 @@
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5399,6 +5386,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización estado recursos en escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -915,19 +915,19 @@
     <t>regreso al autor nuevamente 10/02/2016</t>
   </si>
   <si>
-    <t>proceso 3</t>
-  </si>
-  <si>
-    <t>Listos 28</t>
-  </si>
-  <si>
     <t>Identifica gráficas de funciones</t>
   </si>
   <si>
-    <t>proceso 4</t>
-  </si>
-  <si>
-    <t>faltan 7</t>
+    <t>proceso 6</t>
+  </si>
+  <si>
+    <t>proceso 7</t>
+  </si>
+  <si>
+    <t>faltan 4</t>
+  </si>
+  <si>
+    <t>Listos 31</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1420,16 +1420,40 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1471,29 +1495,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1803,7 +1806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V40" sqref="V40"/>
+      <selection pane="bottomLeft" activeCell="U41" sqref="U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,65 +1838,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="72"/>
-      <c r="O1" s="60" t="s">
+      <c r="N1" s="80"/>
+      <c r="O1" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="P1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="75" t="s">
+      <c r="Q1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="79" t="s">
+      <c r="S1" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="77" t="s">
+      <c r="T1" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="75" t="s">
+      <c r="U1" s="60" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="22" t="s">
@@ -1907,31 +1910,31 @@
       </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="67"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="76"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="61"/>
       <c r="V2" s="9"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2208,7 +2211,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H7" s="52">
         <v>5</v>
@@ -2277,51 +2280,57 @@
         <v>135</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="54">
         <v>6</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12" t="s">
+      <c r="M8" s="53"/>
+      <c r="N8" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="P8" s="13" t="s">
+      <c r="P8" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="54">
         <v>6</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T8" s="41" t="s">
+      <c r="T8" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="U8" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="V8" s="28" t="s">
+      <c r="V8" s="24" t="s">
         <v>252</v>
+      </c>
+      <c r="W8" s="57">
+        <v>42414</v>
+      </c>
+      <c r="X8" s="27">
+        <v>42414</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -3321,51 +3330,57 @@
         <v>135</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="54">
         <v>22</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="J24" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12" t="s">
+      <c r="M24" s="53"/>
+      <c r="N24" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="O24" s="11" t="s">
+      <c r="O24" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="P24" s="13" t="s">
+      <c r="P24" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="13">
+      <c r="Q24" s="54">
         <v>6</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S24" s="14" t="s">
+      <c r="S24" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T24" s="41" t="s">
+      <c r="T24" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="U24" s="13" t="s">
+      <c r="U24" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="V24" s="28" t="s">
+      <c r="V24" s="24" t="s">
         <v>252</v>
+      </c>
+      <c r="W24" s="57">
+        <v>42414</v>
+      </c>
+      <c r="X24" s="27">
+        <v>42414</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4138,51 +4153,57 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="H37" s="42">
+      <c r="H37" s="52">
         <v>35</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="11" t="s">
+      <c r="J37" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K37" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="L37" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12" t="s">
+      <c r="M37" s="53"/>
+      <c r="N37" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="O37" s="11" t="s">
+      <c r="O37" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="P37" s="13" t="s">
+      <c r="P37" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="13">
+      <c r="Q37" s="54">
         <v>6</v>
       </c>
-      <c r="R37" s="13" t="s">
+      <c r="R37" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S37" s="14" t="s">
+      <c r="S37" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T37" s="41" t="s">
+      <c r="T37" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="U37" s="13" t="s">
+      <c r="U37" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="V37" s="29" t="s">
+      <c r="V37" s="83" t="s">
         <v>252</v>
+      </c>
+      <c r="W37" s="57">
+        <v>42414</v>
+      </c>
+      <c r="X37" s="27">
+        <v>42414</v>
       </c>
     </row>
     <row r="38" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4293,7 +4314,7 @@
       <c r="T40" s="14"/>
       <c r="U40" s="13"/>
       <c r="V40" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="W40" t="s">
         <v>259</v>
@@ -4323,10 +4344,10 @@
       <c r="U41" s="44"/>
       <c r="V41" s="46"/>
       <c r="W41" s="47" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="X41" s="48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4352,13 +4373,13 @@
       <c r="T42" s="14"/>
       <c r="U42" s="45"/>
       <c r="V42" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W42" s="47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X42" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -5418,12 +5439,6 @@
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5438,6 +5453,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recurso M para agregar en recurso F
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -1420,6 +1420,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1494,9 +1497,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1804,9 +1804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U41" sqref="U41"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,65 +1838,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="76" t="s">
+      <c r="K1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="80"/>
-      <c r="O1" s="58" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="58" t="s">
+      <c r="P1" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="22" t="s">
@@ -1910,31 +1910,31 @@
       </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="75"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="61"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
       <c r="V2" s="9"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
       <c r="V4" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="W4" s="57">
+      <c r="W4" s="35">
         <v>42412</v>
       </c>
       <c r="X4" s="27">
@@ -2326,7 +2326,7 @@
       <c r="V8" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="W8" s="57">
+      <c r="W8" s="35">
         <v>42414</v>
       </c>
       <c r="X8" s="27">
@@ -4196,7 +4196,7 @@
       <c r="U37" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="V37" s="83" t="s">
+      <c r="V37" s="58" t="s">
         <v>252</v>
       </c>
       <c r="W37" s="57">

</xml_diff>

<commit_message>
Archivos de autor tema MA_08_11_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_MA_08_07_CO.xlsx
@@ -660,9 +660,6 @@
     <t>Evalua tus conocimientos sobre el tema Las funciones</t>
   </si>
   <si>
-    <t>Banco de contenidos: Las funciones</t>
-  </si>
-  <si>
     <t>Fin de unidad</t>
   </si>
   <si>
@@ -928,6 +925,9 @@
   </si>
   <si>
     <t>faltan 3</t>
+  </si>
+  <si>
+    <t>Banco de actividades: Las funciones</t>
   </si>
 </sst>
 </file>
@@ -1420,16 +1420,40 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1469,30 +1493,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1801,9 +1801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,103 +1835,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="72"/>
-      <c r="O1" s="60" t="s">
+      <c r="N1" s="80"/>
+      <c r="O1" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="P1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="75" t="s">
+      <c r="Q1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="79" t="s">
+      <c r="S1" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="77" t="s">
+      <c r="T1" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="75" t="s">
+      <c r="U1" s="60" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="W1" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="X1" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="X1" s="26" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="67"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="76"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="61"/>
       <c r="V2" s="9"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
         <v>123</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -1977,19 +1977,19 @@
         <v>10</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S3" s="39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T3" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U3" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V3" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W3" s="34">
         <v>42394</v>
@@ -2023,7 +2023,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>20</v>
@@ -2045,19 +2045,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S4" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="T4" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T4" s="55" t="s">
+      <c r="U4" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="U4" s="53" t="s">
-        <v>193</v>
-      </c>
       <c r="V4" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W4" s="34">
         <v>42412</v>
@@ -2091,7 +2091,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K5" s="52" t="s">
         <v>20</v>
@@ -2109,19 +2109,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S5" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="T5" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="U5" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="T5" s="55" t="s">
-        <v>203</v>
-      </c>
-      <c r="U5" s="53" t="s">
-        <v>195</v>
-      </c>
       <c r="V5" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="W5" s="56">
         <v>42412</v>
@@ -2177,19 +2177,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="T6" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="U6" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="U6" s="13" t="s">
-        <v>199</v>
-      </c>
       <c r="V6" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H7" s="51">
         <v>5</v>
@@ -2239,19 +2239,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S7" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S7" s="54" t="s">
+      <c r="T7" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T7" s="55" t="s">
+      <c r="U7" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="U7" s="53" t="s">
-        <v>193</v>
-      </c>
       <c r="V7" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W7" s="56">
         <v>42412</v>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H8" s="53">
         <v>6</v>
@@ -2287,7 +2287,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K8" s="52" t="s">
         <v>20</v>
@@ -2309,19 +2309,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S8" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S8" s="54" t="s">
-        <v>191</v>
-      </c>
       <c r="T8" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U8" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W8" s="34">
         <v>42414</v>
@@ -2346,7 +2346,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H9" s="29">
         <v>7</v>
@@ -2355,7 +2355,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K9" s="32" t="s">
         <v>19</v>
@@ -2366,7 +2366,7 @@
       <c r="M9" s="32"/>
       <c r="N9" s="32"/>
       <c r="O9" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P9" s="31" t="s">
         <v>20</v>
@@ -2375,25 +2375,25 @@
         <v>10</v>
       </c>
       <c r="R9" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S9" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="S9" s="33" t="s">
+      <c r="T9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="U9" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="T9" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>184</v>
-      </c>
       <c r="V9" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W9" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X9" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AB9" s="25"/>
     </row>
@@ -2422,7 +2422,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K10" s="32" t="s">
         <v>19</v>
@@ -2442,28 +2442,28 @@
         <v>10</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S10" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T10" s="33" t="s">
         <v>137</v>
       </c>
       <c r="U10" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V10" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W10" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X10" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AB10" s="25"/>
     </row>
@@ -2492,7 +2492,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K11" s="32" t="s">
         <v>19</v>
@@ -2510,25 +2510,25 @@
         <v>10</v>
       </c>
       <c r="R11" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="S11" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="T11" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="S11" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="T11" s="33" t="s">
+      <c r="U11" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="U11" s="31" t="s">
-        <v>218</v>
-      </c>
       <c r="V11" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W11" s="34">
         <v>42395</v>
       </c>
       <c r="X11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2574,25 +2574,25 @@
         <v>10</v>
       </c>
       <c r="R12" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S12" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T12" s="33" t="s">
         <v>139</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W12" s="34">
         <v>42761</v>
       </c>
       <c r="X12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K13" s="32" t="s">
         <v>19</v>
@@ -2638,28 +2638,28 @@
         <v>10</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S13" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T13" s="33" t="s">
         <v>142</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K14" s="32" t="s">
         <v>19</v>
@@ -2705,25 +2705,25 @@
         <v>10</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S14" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T14" s="33" t="s">
         <v>143</v>
       </c>
       <c r="U14" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W14" s="34">
         <v>42395</v>
       </c>
       <c r="X14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K15" s="32" t="s">
         <v>19</v>
@@ -2769,25 +2769,25 @@
         <v>10</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S15" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T15" s="33" t="s">
         <v>144</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W15" s="34">
         <v>42395</v>
       </c>
       <c r="X15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H16" s="31">
         <v>14</v>
@@ -2833,25 +2833,25 @@
         <v>10</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S16" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T16" s="33" t="s">
         <v>145</v>
       </c>
       <c r="U16" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W16" s="34">
         <v>42395</v>
       </c>
       <c r="X16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -2870,7 +2870,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H17" s="29">
         <v>15</v>
@@ -2897,25 +2897,25 @@
         <v>10</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S17" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T17" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U17" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W17" s="34">
         <v>42395</v>
       </c>
       <c r="X17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -2961,28 +2961,28 @@
         <v>10</v>
       </c>
       <c r="R18" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S18" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T18" s="33" t="s">
         <v>148</v>
       </c>
       <c r="U18" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K19" s="32" t="s">
         <v>19</v>
@@ -3028,28 +3028,28 @@
         <v>10</v>
       </c>
       <c r="R19" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S19" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T19" s="33" t="s">
         <v>149</v>
       </c>
       <c r="U19" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H20" s="31">
         <v>18</v>
@@ -3077,7 +3077,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>19</v>
@@ -3095,25 +3095,25 @@
         <v>10</v>
       </c>
       <c r="R20" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="S20" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="T20" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="U20" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="S20" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="T20" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="U20" s="31" t="s">
-        <v>220</v>
-      </c>
       <c r="V20" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W20" s="34">
         <v>42395</v>
       </c>
       <c r="X20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H21" s="29">
         <v>19</v>
@@ -3141,7 +3141,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K21" s="32" t="s">
         <v>19</v>
@@ -3159,25 +3159,25 @@
         <v>10</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S21" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T21" s="33" t="s">
         <v>151</v>
       </c>
       <c r="U21" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V21" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W21" s="34">
         <v>42395</v>
       </c>
       <c r="X21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
       <c r="M22" s="32"/>
       <c r="N22" s="32"/>
       <c r="O22" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P22" s="31" t="s">
         <v>19</v>
@@ -3225,25 +3225,25 @@
         <v>10</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S22" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T22" s="33" t="s">
         <v>152</v>
       </c>
       <c r="U22" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V22" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W22" s="34">
         <v>42395</v>
       </c>
       <c r="X22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H23" s="29">
         <v>21</v>
@@ -3271,7 +3271,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>19</v>
@@ -3289,25 +3289,25 @@
         <v>10</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S23" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T23" s="33" t="s">
         <v>154</v>
       </c>
       <c r="U23" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V23" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W23" s="34">
         <v>42401</v>
       </c>
       <c r="X23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3337,7 +3337,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="50" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K24" s="52" t="s">
         <v>20</v>
@@ -3359,19 +3359,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S24" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S24" s="54" t="s">
-        <v>191</v>
-      </c>
       <c r="T24" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U24" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V24" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W24" s="56">
         <v>42414</v>
@@ -3423,25 +3423,25 @@
         <v>10</v>
       </c>
       <c r="R25" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S25" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="S25" s="33" t="s">
-        <v>183</v>
       </c>
       <c r="T25" s="33" t="s">
         <v>157</v>
       </c>
       <c r="U25" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V25" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W25" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X25" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>19</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K26" s="32" t="s">
         <v>19</v>
@@ -3487,25 +3487,25 @@
         <v>10</v>
       </c>
       <c r="R26" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S26" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="S26" s="33" t="s">
-        <v>183</v>
       </c>
       <c r="T26" s="33" t="s">
         <v>159</v>
       </c>
       <c r="U26" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V26" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W26" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X26" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H27" s="29">
         <v>25</v>
@@ -3533,7 +3533,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K27" s="32" t="s">
         <v>19</v>
@@ -3551,25 +3551,25 @@
         <v>10</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S27" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T27" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U27" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V27" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W27" s="34">
         <v>42402</v>
       </c>
       <c r="X27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H28" s="31">
         <v>26</v>
@@ -3597,7 +3597,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K28" s="32" t="s">
         <v>19</v>
@@ -3615,25 +3615,25 @@
         <v>10</v>
       </c>
       <c r="R28" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S28" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T28" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U28" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V28" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W28" s="34">
         <v>42402</v>
       </c>
       <c r="X28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3679,25 +3679,25 @@
         <v>10</v>
       </c>
       <c r="R29" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S29" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="S29" s="33" t="s">
-        <v>183</v>
       </c>
       <c r="T29" s="33" t="s">
         <v>160</v>
       </c>
       <c r="U29" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V29" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W29" s="34">
         <v>42402</v>
       </c>
       <c r="X29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3747,19 +3747,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="S30" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="S30" s="14" t="s">
-        <v>197</v>
-      </c>
       <c r="T30" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U30" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="V30" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3778,7 +3778,7 @@
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H31" s="29">
         <v>29</v>
@@ -3787,7 +3787,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K31" s="32" t="s">
         <v>19</v>
@@ -3805,25 +3805,25 @@
         <v>10</v>
       </c>
       <c r="R31" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S31" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T31" s="33" t="s">
         <v>162</v>
       </c>
       <c r="U31" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V31" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W31" s="34">
         <v>42403</v>
       </c>
       <c r="X31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3869,25 +3869,25 @@
         <v>10</v>
       </c>
       <c r="R32" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S32" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="S32" s="33" t="s">
-        <v>183</v>
       </c>
       <c r="T32" s="33" t="s">
         <v>163</v>
       </c>
       <c r="U32" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V32" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W32" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X32" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="N33" s="12"/>
       <c r="O33" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P33" s="13" t="s">
         <v>20</v>
@@ -3937,22 +3937,22 @@
         <v>6</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S33" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="T33" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="U33" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="T33" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="U33" s="13" t="s">
-        <v>195</v>
-      </c>
       <c r="V33" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4000,25 +4000,25 @@
         <v>10</v>
       </c>
       <c r="R34" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S34" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="S34" s="33" t="s">
+      <c r="T34" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="U34" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="T34" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="U34" s="31" t="s">
-        <v>184</v>
-      </c>
       <c r="V34" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W34" s="34">
         <v>42402</v>
       </c>
       <c r="X34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4037,7 +4037,7 @@
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H35" s="29">
         <v>33</v>
@@ -4046,7 +4046,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K35" s="32" t="s">
         <v>19</v>
@@ -4064,25 +4064,25 @@
         <v>10</v>
       </c>
       <c r="R35" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S35" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T35" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U35" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V35" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W35" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4096,7 +4096,7 @@
         <v>123</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -4132,7 +4132,7 @@
       <c r="V36" s="42"/>
       <c r="W36" s="42"/>
       <c r="X36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
         <v>123</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
@@ -4173,7 +4173,7 @@
         <v>33</v>
       </c>
       <c r="O37" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P37" s="53" t="s">
         <v>19</v>
@@ -4182,19 +4182,19 @@
         <v>6</v>
       </c>
       <c r="R37" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S37" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S37" s="54" t="s">
+      <c r="T37" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="T37" s="55" t="s">
+      <c r="U37" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="U37" s="53" t="s">
-        <v>193</v>
-      </c>
       <c r="V37" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W37" s="56">
         <v>42414</v>
@@ -4214,12 +4214,12 @@
         <v>123</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="50" t="s">
-        <v>176</v>
+        <v>265</v>
       </c>
       <c r="H38" s="53">
         <v>36</v>
@@ -4228,7 +4228,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K38" s="52" t="s">
         <v>20</v>
@@ -4241,7 +4241,7 @@
         <v>52</v>
       </c>
       <c r="O38" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P38" s="53" t="s">
         <v>20</v>
@@ -4250,19 +4250,19 @@
         <v>6</v>
       </c>
       <c r="R38" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="S38" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="S38" s="54" t="s">
-        <v>191</v>
-      </c>
       <c r="T38" s="55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U38" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V38" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W38" s="56">
         <v>42415</v>
@@ -4317,10 +4317,10 @@
       <c r="T40" s="14"/>
       <c r="U40" s="13"/>
       <c r="V40" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="W40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4347,10 +4347,10 @@
       <c r="U41" s="43"/>
       <c r="V41" s="45"/>
       <c r="W41" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X41" s="47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4376,13 +4376,13 @@
       <c r="T42" s="14"/>
       <c r="U42" s="44"/>
       <c r="V42" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W42" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X42" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -4396,7 +4396,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="12"/>
       <c r="J43" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
@@ -4421,7 +4421,7 @@
       <c r="H44" s="11"/>
       <c r="I44" s="12"/>
       <c r="J44" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
@@ -5442,12 +5442,6 @@
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5462,6 +5456,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>